<commit_message>
Excel calculator + Readme
</commit_message>
<xml_diff>
--- a/GSS15 - Excel Calculator.xlsx
+++ b/GSS15 - Excel Calculator.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\userMN\M\mann0242\MyWork\GitHub\GSS-15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B4755DE0-A226-4C18-BB03-DCBE615F7D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06095FF4-4104-4866-AD03-2CF1931F2D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GSS15 - Excel Calculator" sheetId="1" r:id="rId1"/>
     <sheet name="raw_data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -153,7 +166,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,18 +724,65 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -740,7 +800,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -754,6 +814,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -762,6 +823,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -770,6 +832,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -778,6 +841,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -794,6 +858,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -802,71 +867,30 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -882,57 +906,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q4" totalsRowShown="0">
-  <autoFilter ref="A1:Q4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:Q4" totalsRowShown="0">
+  <autoFilter ref="A1:Q4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="participant_id" dataDxfId="0"/>
-    <tableColumn id="2" name="q4_recoded" dataDxfId="1">
-      <calculatedColumnFormula>IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;300, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;360, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;=420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;=480), 3, "Bad duration number!"))))</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="participant_id" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="q4_recoded" dataDxfId="15">
+      <calculatedColumnFormula>IF(ISBLANK(data[[#This Row],[question_4]]), "", IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;300, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;360, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;=420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;=480), 3, "Bad duration number!")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="q7_recoded" dataDxfId="10">
-      <calculatedColumnFormula>IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;300, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;360, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;=420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;=480), 3, "Bad duration number!"))))</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="q7_recoded" dataDxfId="14">
+      <calculatedColumnFormula>IF(ISBLANK(data[[#This Row],[question_7]]), "", IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;300, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;360, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;=420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;=480), 3, "Bad duration number!")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="q8_recoded" dataDxfId="9">
-      <calculatedColumnFormula>IF(OR(data[[#This Row],[question_8]]=0, data[[#This Row],[question_8]]=5), 0, IF(OR(data[[#This Row],[question_8]]=1, data[[#This Row],[question_8]]=4), 1, IF(OR(data[[#This Row],[question_8]]=2, data[[#This Row],[question_8]]=3), 2, "Bad Q8 number")))</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="q8_recoded" dataDxfId="13">
+      <calculatedColumnFormula>IF(ISBLANK(data[[#This Row],[question_8]]), "", IF(OR(data[[#This Row],[question_8]]=0, data[[#This Row],[question_8]]=5), 0, IF(OR(data[[#This Row],[question_8]]=1, data[[#This Row],[question_8]]=4), 1, IF(OR(data[[#This Row],[question_8]]=2, data[[#This Row],[question_8]]=3), 2, "Bad Q8 number"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="q9_recoded" dataDxfId="8">
-      <calculatedColumnFormula>IF(OR(data[[#This Row],[question_9]]=0, data[[#This Row],[question_9]]=3), 0, IF(OR(data[[#This Row],[question_9]]=1, data[[#This Row],[question_9]]=2), 1, "Bad Q9 number"))</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="q9_recoded" dataDxfId="12">
+      <calculatedColumnFormula>IF(ISBLANK(data[[#This Row],[question_9]]), "", IF(OR(data[[#This Row],[question_9]]=0, data[[#This Row],[question_9]]=3), 0, IF(OR(data[[#This Row],[question_9]]=1, data[[#This Row],[question_9]]=2), 1, "Bad Q9 number")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="weekday_mp" dataDxfId="7">
-      <calculatedColumnFormula>MOD((HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]])) + ((HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) + IF(HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) &lt; HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]), 1440, 0) - (HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]))) / 2), 1440)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="weekday_mp" dataDxfId="11">
+      <calculatedColumnFormula>IF(OR(ISBLANK(data[[#This Row],[question_2]]), ISBLANK(data[[#This Row],[question_3]])), "", MOD((HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]])) + ((HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) + IF(HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) &lt; HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]), 1440, 0) - (HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]))) / 2), 1440))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="weekend_mp" dataDxfId="6">
-      <calculatedColumnFormula>MOD((HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]])) + ((HOUR(data[[#This Row],[question_6]])*60 + MINUTE(data[[#This Row],[question_6]]) + IF(HOUR(data[[#This Row],[question_6]])*60 + MINUTE(data[[#This Row],[question_6]]) &lt; HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]]), 1440, 0) - (HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]]))) / 2), 1440)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="weekend_mp" dataDxfId="10">
+      <calculatedColumnFormula>IF(OR(ISBLANK(data[[#This Row],[question_5]]),ISBLANK(data[[#This Row],[question_6]])),"",MOD((HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]]))+((HOUR(data[[#This Row],[question_6]])*60+MINUTE(data[[#This Row],[question_6]])+IF(HOUR(data[[#This Row],[question_6]])*60+MINUTE(data[[#This Row],[question_6]])&lt;HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]]),1440,0)-(HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]])))/2),1440))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="midpoint_score" dataDxfId="5">
-      <calculatedColumnFormula>IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=45, Table2[[#This Row],[weekday_mp]]&gt;=255), 0, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=60, Table2[[#This Row],[weekday_mp]]&gt;=240), 1, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=75, Table2[[#This Row],[weekday_mp]]&gt;=225), 2, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=90, Table2[[#This Row],[weekday_mp]]&gt;=210), 3, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=105, Table2[[#This Row],[weekday_mp]]&gt;=195), 4, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=120, Table2[[#This Row],[weekday_mp]]&gt;=180), 5, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=135, Table2[[#This Row],[weekday_mp]]&gt;=165), 6, 7)))))))</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="midpoint_score" dataDxfId="9">
+      <calculatedColumnFormula>IF(ISBLANK(Table2[[#This Row],[weekday_mp]]), "", IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=45, Table2[[#This Row],[weekday_mp]]&gt;=255), 0, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=60, Table2[[#This Row],[weekday_mp]]&gt;=240), 1, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=75, Table2[[#This Row],[weekday_mp]]&gt;=225), 2, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=90, Table2[[#This Row],[weekday_mp]]&gt;=210), 3, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=105, Table2[[#This Row],[weekday_mp]]&gt;=195), 4, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=120, Table2[[#This Row],[weekday_mp]]&gt;=180), 5, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=135, Table2[[#This Row],[weekday_mp]]&gt;=165), 6, 7))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="social_jetlag_score" dataDxfId="4">
-      <calculatedColumnFormula array="1">_xlfn.IFS(ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=90, 0, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=60, 1, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=30, 2, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&lt;30, 3)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="social_jetlag_score" dataDxfId="8">
+      <calculatedColumnFormula array="1">IF(OR(ISBLANK(Table2[[#This Row],[weekday_mp]]), ISBLANK(Table2[[#This Row],[weekend_mp]])), "", _xlfn.IFS(ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=90, 0, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=60, 1, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=30, 2, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&lt;30, 3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="sleep_duration_discrepancy_score" dataDxfId="2">
-      <calculatedColumnFormula array="1">_xlfn.IFS(ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=120, 0, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=90, 1, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=60, 2, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=30, 3, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&lt;30, 4)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="sleep_duration_discrepancy_score" dataDxfId="7">
+      <calculatedColumnFormula array="1">IF(OR(ISBLANK(data[[#This Row],[question_4]]),ISBLANK(data[[#This Row],[question_7]])),"",_xlfn.IFS(ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=120, 0, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=90, 1, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=60, 2, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=30, 3, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&lt;30, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="problem_score" dataDxfId="3">
-      <calculatedColumnFormula array="1">_xlfn.IFS(data[[#This Row],[question_1]]=0, 0, data[[#This Row],[question_1]]=1, 10, data[[#This Row],[question_1]]=2, 5)</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="problem_score" dataDxfId="6">
+      <calculatedColumnFormula array="1">IF(ISBLANK(data[[#This Row],[question_1]]), "", _xlfn.IFS(data[[#This Row],[question_1]]=0, 0, data[[#This Row],[question_1]]=1, 10, data[[#This Row],[question_1]]=2, 5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="duration_score" dataDxfId="16">
-      <calculatedColumnFormula>Table2[[#This Row],[q4_recoded]]+Table2[[#This Row],[q7_recoded]]</calculatedColumnFormula>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="duration_score" dataDxfId="0">
+      <calculatedColumnFormula>IF(COUNTA(Table2[[#This Row],[q4_recoded]], Table2[[#This Row],[q7_recoded]])=2, Table2[[#This Row],[q4_recoded]] + Table2[[#This Row],[q7_recoded]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="timing_score" dataDxfId="15">
-      <calculatedColumnFormula>Table2[[#This Row],[q8_recoded]]+Table2[[#This Row],[q9_recoded]]+Table2[[#This Row],[midpoint_score]]</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="timing_score" dataDxfId="1">
+      <calculatedColumnFormula>IF(COUNTA(Table2[[#This Row],[q8_recoded]], Table2[[#This Row],[q9_recoded]], Table2[[#This Row],[midpoint_score]])=3, Table2[[#This Row],[q8_recoded]] + Table2[[#This Row],[q9_recoded]] + Table2[[#This Row],[midpoint_score]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="regularity_score" dataDxfId="14">
-      <calculatedColumnFormula>Table2[[#This Row],[social_jetlag_score]]+Table2[[#This Row],[sleep_duration_discrepancy_score]]</calculatedColumnFormula>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="regularity_score" dataDxfId="3">
+      <calculatedColumnFormula>IF(COUNTA(Table2[[#This Row],[social_jetlag_score]], Table2[[#This Row],[sleep_duration_discrepancy_score]])=2, Table2[[#This Row],[social_jetlag_score]] + Table2[[#This Row],[sleep_duration_discrepancy_score]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="adequacy_score" dataDxfId="13">
-      <calculatedColumnFormula>(data[[#This Row],[question_10]])+(data[[#This Row],[question_14]])+(3-data[[#This Row],[question_15]])</calculatedColumnFormula>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="adequacy_score" dataDxfId="2">
+      <calculatedColumnFormula>IF(COUNTA(data[[#This Row],[question_10]], data[[#This Row],[question_14]], data[[#This Row],[question_15]])=3, (data[[#This Row],[question_10]]) + (data[[#This Row],[question_14]]) + (3-data[[#This Row],[question_15]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="insomnia_score" dataDxfId="11">
-      <calculatedColumnFormula>(3-data[[#This Row],[question_11]])+(3-data[[#This Row],[question_12]])+(3-data[[#This Row],[question_13]])</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="insomnia_score" dataDxfId="4">
+      <calculatedColumnFormula>IF(COUNTA(data[[#This Row],[question_11]], data[[#This Row],[question_12]], data[[#This Row],[question_13]])=3, (3-data[[#This Row],[question_11]]) + (3-data[[#This Row],[question_12]]) + (3-data[[#This Row],[question_13]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="total_score" dataDxfId="12">
-      <calculatedColumnFormula>Table2[[#This Row],[problem_score]]+Table2[[#This Row],[duration_score]]+Table2[[#This Row],[timing_score]]+Table2[[#This Row],[regularity_score]]+Table2[[#This Row],[adequacy_score]]+Table2[[#This Row],[insomnia_score]]</calculatedColumnFormula>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="total_score" dataDxfId="5">
+      <calculatedColumnFormula>IF(COUNTA(Table2[[#This Row],[problem_score]], Table2[[#This Row],[duration_score]], Table2[[#This Row],[timing_score]], Table2[[#This Row],[regularity_score]], Table2[[#This Row],[adequacy_score]], Table2[[#This Row],[insomnia_score]])=6, Table2[[#This Row],[problem_score]]+Table2[[#This Row],[duration_score]]+Table2[[#This Row],[timing_score]]+Table2[[#This Row],[regularity_score]]+Table2[[#This Row],[adequacy_score]]+Table2[[#This Row],[insomnia_score]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -940,25 +964,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="data" displayName="data" ref="A1:P4" totalsRowShown="0">
-  <autoFilter ref="A1:P4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="data" displayName="data" ref="A1:P4" totalsRowShown="0">
+  <autoFilter ref="A1:P4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="participant_id"/>
-    <tableColumn id="2" name="question_1"/>
-    <tableColumn id="3" name="question_2" dataDxfId="22"/>
-    <tableColumn id="4" name="question_3" dataDxfId="21"/>
-    <tableColumn id="5" name="question_4" dataDxfId="20"/>
-    <tableColumn id="6" name="question_5" dataDxfId="19"/>
-    <tableColumn id="7" name="question_6" dataDxfId="18"/>
-    <tableColumn id="8" name="question_7" dataDxfId="17"/>
-    <tableColumn id="9" name="question_8"/>
-    <tableColumn id="10" name="question_9"/>
-    <tableColumn id="11" name="question_10"/>
-    <tableColumn id="12" name="question_11"/>
-    <tableColumn id="13" name="question_12"/>
-    <tableColumn id="14" name="question_13"/>
-    <tableColumn id="15" name="question_14"/>
-    <tableColumn id="16" name="question_15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="participant_id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="question_1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="question_2" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="question_3" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="question_4" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="question_5" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="question_6" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="question_7" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="question_8"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="question_9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="question_10"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="question_11"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="question_12"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="question_13"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="question_14"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="question_15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1260,11 +1284,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,67 +1361,67 @@
         <v>17</v>
       </c>
       <c r="B2" s="5">
-        <f>IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;300, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;360, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;=420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;=480), 3, "Bad duration number!"))))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_4]]), "", IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;300, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;360, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;=420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;=480), 3, "Bad duration number!")))))</f>
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <f>IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;300, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;360, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;=420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;=480), 3, "Bad duration number!"))))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_7]]), "", IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;300, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;360, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;=420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;=480), 3, "Bad duration number!")))))</f>
         <v>3</v>
       </c>
       <c r="D2" s="5">
-        <f>IF(OR(data[[#This Row],[question_8]]=0, data[[#This Row],[question_8]]=5), 0, IF(OR(data[[#This Row],[question_8]]=1, data[[#This Row],[question_8]]=4), 1, IF(OR(data[[#This Row],[question_8]]=2, data[[#This Row],[question_8]]=3), 2, "Bad Q8 number")))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_8]]), "", IF(OR(data[[#This Row],[question_8]]=0, data[[#This Row],[question_8]]=5), 0, IF(OR(data[[#This Row],[question_8]]=1, data[[#This Row],[question_8]]=4), 1, IF(OR(data[[#This Row],[question_8]]=2, data[[#This Row],[question_8]]=3), 2, "Bad Q8 number"))))</f>
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <f>IF(OR(data[[#This Row],[question_9]]=0, data[[#This Row],[question_9]]=3), 0, IF(OR(data[[#This Row],[question_9]]=1, data[[#This Row],[question_9]]=2), 1, "Bad Q9 number"))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_9]]), "", IF(OR(data[[#This Row],[question_9]]=0, data[[#This Row],[question_9]]=3), 0, IF(OR(data[[#This Row],[question_9]]=1, data[[#This Row],[question_9]]=2), 1, "Bad Q9 number")))</f>
         <v>0</v>
       </c>
       <c r="F2" s="5">
-        <f>MOD((HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]])) + ((HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) + IF(HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) &lt; HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]), 1440, 0) - (HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]))) / 2), 1440)</f>
+        <f>IF(OR(ISBLANK(data[[#This Row],[question_2]]), ISBLANK(data[[#This Row],[question_3]])), "", MOD((HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]])) + ((HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) + IF(HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) &lt; HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]), 1440, 0) - (HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]))) / 2), 1440))</f>
         <v>120</v>
       </c>
       <c r="G2" s="5">
-        <f>MOD((HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]])) + ((HOUR(data[[#This Row],[question_6]])*60 + MINUTE(data[[#This Row],[question_6]]) + IF(HOUR(data[[#This Row],[question_6]])*60 + MINUTE(data[[#This Row],[question_6]]) &lt; HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]]), 1440, 0) - (HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]]))) / 2), 1440)</f>
+        <f>IF(OR(ISBLANK(data[[#This Row],[question_5]]),ISBLANK(data[[#This Row],[question_6]])),"",MOD((HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]]))+((HOUR(data[[#This Row],[question_6]])*60+MINUTE(data[[#This Row],[question_6]])+IF(HOUR(data[[#This Row],[question_6]])*60+MINUTE(data[[#This Row],[question_6]])&lt;HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]]),1440,0)-(HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]])))/2),1440))</f>
         <v>180</v>
       </c>
       <c r="H2" s="5">
-        <f>IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=45, Table2[[#This Row],[weekday_mp]]&gt;=255), 0, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=60, Table2[[#This Row],[weekday_mp]]&gt;=240), 1, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=75, Table2[[#This Row],[weekday_mp]]&gt;=225), 2, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=90, Table2[[#This Row],[weekday_mp]]&gt;=210), 3, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=105, Table2[[#This Row],[weekday_mp]]&gt;=195), 4, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=120, Table2[[#This Row],[weekday_mp]]&gt;=180), 5, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=135, Table2[[#This Row],[weekday_mp]]&gt;=165), 6, 7)))))))</f>
+        <f>IF(ISBLANK(Table2[[#This Row],[weekday_mp]]), "", IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=45, Table2[[#This Row],[weekday_mp]]&gt;=255), 0, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=60, Table2[[#This Row],[weekday_mp]]&gt;=240), 1, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=75, Table2[[#This Row],[weekday_mp]]&gt;=225), 2, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=90, Table2[[#This Row],[weekday_mp]]&gt;=210), 3, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=105, Table2[[#This Row],[weekday_mp]]&gt;=195), 4, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=120, Table2[[#This Row],[weekday_mp]]&gt;=180), 5, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=135, Table2[[#This Row],[weekday_mp]]&gt;=165), 6, 7))))))))</f>
         <v>5</v>
       </c>
       <c r="I2" s="5" cm="1">
-        <f t="array" ref="I2">_xlfn.IFS(ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=90, 0, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=60, 1, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=30, 2, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&lt;30, 3)</f>
+        <f t="array" ref="I2">IF(OR(ISBLANK(Table2[[#This Row],[weekday_mp]]), ISBLANK(Table2[[#This Row],[weekend_mp]])), "", _xlfn.IFS(ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=90, 0, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=60, 1, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=30, 2, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&lt;30, 3))</f>
         <v>1</v>
       </c>
       <c r="J2" s="6" cm="1">
-        <f t="array" ref="J2">_xlfn.IFS(ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=120, 0, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=90, 1, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=60, 2, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=30, 3, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&lt;30, 4)</f>
+        <f t="array" ref="J2">IF(OR(ISBLANK(data[[#This Row],[question_4]]),ISBLANK(data[[#This Row],[question_7]])),"",_xlfn.IFS(ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=120, 0, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=90, 1, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=60, 2, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=30, 3, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&lt;30, 4))</f>
         <v>2</v>
       </c>
       <c r="K2" s="3" cm="1">
-        <f t="array" ref="K2">_xlfn.IFS(data[[#This Row],[question_1]]=0, 0, data[[#This Row],[question_1]]=1, 10, data[[#This Row],[question_1]]=2, 5)</f>
+        <f t="array" ref="K2">IF(ISBLANK(data[[#This Row],[question_1]]), "", _xlfn.IFS(data[[#This Row],[question_1]]=0, 0, data[[#This Row],[question_1]]=1, 10, data[[#This Row],[question_1]]=2, 5))</f>
         <v>5</v>
       </c>
       <c r="L2" s="3">
-        <f>Table2[[#This Row],[q4_recoded]]+Table2[[#This Row],[q7_recoded]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[q4_recoded]], Table2[[#This Row],[q7_recoded]])=2, Table2[[#This Row],[q4_recoded]] + Table2[[#This Row],[q7_recoded]], "")</f>
         <v>5</v>
       </c>
       <c r="M2" s="3">
-        <f>Table2[[#This Row],[q8_recoded]]+Table2[[#This Row],[q9_recoded]]+Table2[[#This Row],[midpoint_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[q8_recoded]], Table2[[#This Row],[q9_recoded]], Table2[[#This Row],[midpoint_score]])=3, Table2[[#This Row],[q8_recoded]] + Table2[[#This Row],[q9_recoded]] + Table2[[#This Row],[midpoint_score]], "")</f>
         <v>6</v>
       </c>
       <c r="N2" s="4">
-        <f>Table2[[#This Row],[social_jetlag_score]]+Table2[[#This Row],[sleep_duration_discrepancy_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[social_jetlag_score]], Table2[[#This Row],[sleep_duration_discrepancy_score]])=2, Table2[[#This Row],[social_jetlag_score]] + Table2[[#This Row],[sleep_duration_discrepancy_score]], "")</f>
         <v>3</v>
       </c>
       <c r="O2" s="3">
-        <f>(data[[#This Row],[question_10]])+(data[[#This Row],[question_14]])+(3-data[[#This Row],[question_15]])</f>
+        <f>IF(COUNTA(data[[#This Row],[question_10]], data[[#This Row],[question_14]], data[[#This Row],[question_15]])=3, (data[[#This Row],[question_10]]) + (data[[#This Row],[question_14]]) + (3-data[[#This Row],[question_15]]), "")</f>
         <v>5</v>
       </c>
       <c r="P2" s="3">
-        <f>(3-data[[#This Row],[question_11]])+(3-data[[#This Row],[question_12]])+(3-data[[#This Row],[question_13]])</f>
+        <f>IF(COUNTA(data[[#This Row],[question_11]], data[[#This Row],[question_12]], data[[#This Row],[question_13]])=3, (3-data[[#This Row],[question_11]]) + (3-data[[#This Row],[question_12]]) + (3-data[[#This Row],[question_13]]), "")</f>
         <v>6</v>
       </c>
       <c r="Q2" s="2">
-        <f>Table2[[#This Row],[problem_score]]+Table2[[#This Row],[duration_score]]+Table2[[#This Row],[timing_score]]+Table2[[#This Row],[regularity_score]]+Table2[[#This Row],[adequacy_score]]+Table2[[#This Row],[insomnia_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[problem_score]], Table2[[#This Row],[duration_score]], Table2[[#This Row],[timing_score]], Table2[[#This Row],[regularity_score]], Table2[[#This Row],[adequacy_score]], Table2[[#This Row],[insomnia_score]])=6, Table2[[#This Row],[problem_score]]+Table2[[#This Row],[duration_score]]+Table2[[#This Row],[timing_score]]+Table2[[#This Row],[regularity_score]]+Table2[[#This Row],[adequacy_score]]+Table2[[#This Row],[insomnia_score]], "")</f>
         <v>30</v>
       </c>
     </row>
@@ -1406,67 +1430,67 @@
         <v>18</v>
       </c>
       <c r="B3" s="5">
-        <f>IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;300, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;360, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;=420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;=480), 3, "Bad duration number!"))))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_4]]), "", IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;300, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;360, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;=420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;=480), 3, "Bad duration number!")))))</f>
         <v>3</v>
       </c>
       <c r="C3" s="5">
-        <f>IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;300, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;360, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;=420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;=480), 3, "Bad duration number!"))))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_7]]), "", IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;300, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;360, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;=420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;=480), 3, "Bad duration number!")))))</f>
         <v>3</v>
       </c>
       <c r="D3" s="5">
-        <f>IF(OR(data[[#This Row],[question_8]]=0, data[[#This Row],[question_8]]=5), 0, IF(OR(data[[#This Row],[question_8]]=1, data[[#This Row],[question_8]]=4), 1, IF(OR(data[[#This Row],[question_8]]=2, data[[#This Row],[question_8]]=3), 2, "Bad Q8 number")))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_8]]), "", IF(OR(data[[#This Row],[question_8]]=0, data[[#This Row],[question_8]]=5), 0, IF(OR(data[[#This Row],[question_8]]=1, data[[#This Row],[question_8]]=4), 1, IF(OR(data[[#This Row],[question_8]]=2, data[[#This Row],[question_8]]=3), 2, "Bad Q8 number"))))</f>
         <v>2</v>
       </c>
       <c r="E3" s="5">
-        <f>IF(OR(data[[#This Row],[question_9]]=0, data[[#This Row],[question_9]]=3), 0, IF(OR(data[[#This Row],[question_9]]=1, data[[#This Row],[question_9]]=2), 1, "Bad Q9 number"))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_9]]), "", IF(OR(data[[#This Row],[question_9]]=0, data[[#This Row],[question_9]]=3), 0, IF(OR(data[[#This Row],[question_9]]=1, data[[#This Row],[question_9]]=2), 1, "Bad Q9 number")))</f>
         <v>1</v>
       </c>
       <c r="F3" s="5">
-        <f>MOD((HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]])) + ((HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) + IF(HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) &lt; HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]), 1440, 0) - (HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]))) / 2), 1440)</f>
+        <f>IF(OR(ISBLANK(data[[#This Row],[question_2]]), ISBLANK(data[[#This Row],[question_3]])), "", MOD((HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]])) + ((HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) + IF(HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) &lt; HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]), 1440, 0) - (HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]))) / 2), 1440))</f>
         <v>150</v>
       </c>
       <c r="G3" s="5">
-        <f>MOD((HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]])) + ((HOUR(data[[#This Row],[question_6]])*60 + MINUTE(data[[#This Row],[question_6]]) + IF(HOUR(data[[#This Row],[question_6]])*60 + MINUTE(data[[#This Row],[question_6]]) &lt; HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]]), 1440, 0) - (HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]]))) / 2), 1440)</f>
+        <f>IF(OR(ISBLANK(data[[#This Row],[question_5]]),ISBLANK(data[[#This Row],[question_6]])),"",MOD((HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]]))+((HOUR(data[[#This Row],[question_6]])*60+MINUTE(data[[#This Row],[question_6]])+IF(HOUR(data[[#This Row],[question_6]])*60+MINUTE(data[[#This Row],[question_6]])&lt;HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]]),1440,0)-(HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]])))/2),1440))</f>
         <v>150</v>
       </c>
       <c r="H3" s="5">
-        <f>IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=45, Table2[[#This Row],[weekday_mp]]&gt;=255), 0, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=60, Table2[[#This Row],[weekday_mp]]&gt;=240), 1, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=75, Table2[[#This Row],[weekday_mp]]&gt;=225), 2, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=90, Table2[[#This Row],[weekday_mp]]&gt;=210), 3, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=105, Table2[[#This Row],[weekday_mp]]&gt;=195), 4, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=120, Table2[[#This Row],[weekday_mp]]&gt;=180), 5, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=135, Table2[[#This Row],[weekday_mp]]&gt;=165), 6, 7)))))))</f>
+        <f>IF(ISBLANK(Table2[[#This Row],[weekday_mp]]), "", IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=45, Table2[[#This Row],[weekday_mp]]&gt;=255), 0, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=60, Table2[[#This Row],[weekday_mp]]&gt;=240), 1, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=75, Table2[[#This Row],[weekday_mp]]&gt;=225), 2, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=90, Table2[[#This Row],[weekday_mp]]&gt;=210), 3, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=105, Table2[[#This Row],[weekday_mp]]&gt;=195), 4, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=120, Table2[[#This Row],[weekday_mp]]&gt;=180), 5, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=135, Table2[[#This Row],[weekday_mp]]&gt;=165), 6, 7))))))))</f>
         <v>7</v>
       </c>
       <c r="I3" s="5" cm="1">
-        <f t="array" ref="I3">_xlfn.IFS(ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=90, 0, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=60, 1, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=30, 2, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&lt;30, 3)</f>
+        <f t="array" ref="I3">IF(OR(ISBLANK(Table2[[#This Row],[weekday_mp]]), ISBLANK(Table2[[#This Row],[weekend_mp]])), "", _xlfn.IFS(ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=90, 0, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=60, 1, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=30, 2, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&lt;30, 3))</f>
         <v>3</v>
       </c>
       <c r="J3" s="6" cm="1">
-        <f t="array" ref="J3">_xlfn.IFS(ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=120, 0, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=90, 1, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=60, 2, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=30, 3, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&lt;30, 4)</f>
+        <f t="array" ref="J3">IF(OR(ISBLANK(data[[#This Row],[question_4]]),ISBLANK(data[[#This Row],[question_7]])),"",_xlfn.IFS(ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=120, 0, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=90, 1, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=60, 2, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=30, 3, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&lt;30, 4))</f>
         <v>4</v>
       </c>
       <c r="K3" s="3" cm="1">
-        <f t="array" ref="K3">_xlfn.IFS(data[[#This Row],[question_1]]=0, 0, data[[#This Row],[question_1]]=1, 10, data[[#This Row],[question_1]]=2, 5)</f>
+        <f t="array" ref="K3">IF(ISBLANK(data[[#This Row],[question_1]]), "", _xlfn.IFS(data[[#This Row],[question_1]]=0, 0, data[[#This Row],[question_1]]=1, 10, data[[#This Row],[question_1]]=2, 5))</f>
         <v>10</v>
       </c>
       <c r="L3" s="3">
-        <f>Table2[[#This Row],[q4_recoded]]+Table2[[#This Row],[q7_recoded]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[q4_recoded]], Table2[[#This Row],[q7_recoded]])=2, Table2[[#This Row],[q4_recoded]] + Table2[[#This Row],[q7_recoded]], "")</f>
         <v>6</v>
       </c>
       <c r="M3" s="3">
-        <f>Table2[[#This Row],[q8_recoded]]+Table2[[#This Row],[q9_recoded]]+Table2[[#This Row],[midpoint_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[q8_recoded]], Table2[[#This Row],[q9_recoded]], Table2[[#This Row],[midpoint_score]])=3, Table2[[#This Row],[q8_recoded]] + Table2[[#This Row],[q9_recoded]] + Table2[[#This Row],[midpoint_score]], "")</f>
         <v>10</v>
       </c>
       <c r="N3" s="4">
-        <f>Table2[[#This Row],[social_jetlag_score]]+Table2[[#This Row],[sleep_duration_discrepancy_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[social_jetlag_score]], Table2[[#This Row],[sleep_duration_discrepancy_score]])=2, Table2[[#This Row],[social_jetlag_score]] + Table2[[#This Row],[sleep_duration_discrepancy_score]], "")</f>
         <v>7</v>
       </c>
       <c r="O3" s="3">
-        <f>(data[[#This Row],[question_10]])+(data[[#This Row],[question_14]])+(3-data[[#This Row],[question_15]])</f>
+        <f>IF(COUNTA(data[[#This Row],[question_10]], data[[#This Row],[question_14]], data[[#This Row],[question_15]])=3, (data[[#This Row],[question_10]]) + (data[[#This Row],[question_14]]) + (3-data[[#This Row],[question_15]]), "")</f>
         <v>10</v>
       </c>
       <c r="P3" s="3">
-        <f>(3-data[[#This Row],[question_11]])+(3-data[[#This Row],[question_12]])+(3-data[[#This Row],[question_13]])</f>
+        <f>IF(COUNTA(data[[#This Row],[question_11]], data[[#This Row],[question_12]], data[[#This Row],[question_13]])=3, (3-data[[#This Row],[question_11]]) + (3-data[[#This Row],[question_12]]) + (3-data[[#This Row],[question_13]]), "")</f>
         <v>9</v>
       </c>
       <c r="Q3" s="2">
-        <f>Table2[[#This Row],[problem_score]]+Table2[[#This Row],[duration_score]]+Table2[[#This Row],[timing_score]]+Table2[[#This Row],[regularity_score]]+Table2[[#This Row],[adequacy_score]]+Table2[[#This Row],[insomnia_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[problem_score]], Table2[[#This Row],[duration_score]], Table2[[#This Row],[timing_score]], Table2[[#This Row],[regularity_score]], Table2[[#This Row],[adequacy_score]], Table2[[#This Row],[insomnia_score]])=6, Table2[[#This Row],[problem_score]]+Table2[[#This Row],[duration_score]]+Table2[[#This Row],[timing_score]]+Table2[[#This Row],[regularity_score]]+Table2[[#This Row],[adequacy_score]]+Table2[[#This Row],[insomnia_score]], "")</f>
         <v>52</v>
       </c>
     </row>
@@ -1475,67 +1499,67 @@
         <v>19</v>
       </c>
       <c r="B4" s="5">
-        <f>IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;300, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;360, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;=420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;=480), 3, "Bad duration number!"))))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_4]]), "", IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;300, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;360, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&gt;=420, HOUR(data[[#This Row],[question_4]])*60 + MINUTE(data[[#This Row],[question_4]])&lt;=480), 3, "Bad duration number!")))))</f>
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <f>IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;300, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;360, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;=420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;=480), 3, "Bad duration number!"))))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_7]]), "", IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;300, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;600), 0, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;360, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;540), 1, IF(OR(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;480), 2, IF(AND(HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&gt;=420, HOUR(data[[#This Row],[question_7]])*60 + MINUTE(data[[#This Row],[question_7]])&lt;=480), 3, "Bad duration number!")))))</f>
         <v>0</v>
       </c>
       <c r="D4" s="5">
-        <f>IF(OR(data[[#This Row],[question_8]]=0, data[[#This Row],[question_8]]=5), 0, IF(OR(data[[#This Row],[question_8]]=1, data[[#This Row],[question_8]]=4), 1, IF(OR(data[[#This Row],[question_8]]=2, data[[#This Row],[question_8]]=3), 2, "Bad Q8 number")))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_8]]), "", IF(OR(data[[#This Row],[question_8]]=0, data[[#This Row],[question_8]]=5), 0, IF(OR(data[[#This Row],[question_8]]=1, data[[#This Row],[question_8]]=4), 1, IF(OR(data[[#This Row],[question_8]]=2, data[[#This Row],[question_8]]=3), 2, "Bad Q8 number"))))</f>
         <v>0</v>
       </c>
       <c r="E4" s="5">
-        <f>IF(OR(data[[#This Row],[question_9]]=0, data[[#This Row],[question_9]]=3), 0, IF(OR(data[[#This Row],[question_9]]=1, data[[#This Row],[question_9]]=2), 1, "Bad Q9 number"))</f>
+        <f>IF(ISBLANK(data[[#This Row],[question_9]]), "", IF(OR(data[[#This Row],[question_9]]=0, data[[#This Row],[question_9]]=3), 0, IF(OR(data[[#This Row],[question_9]]=1, data[[#This Row],[question_9]]=2), 1, "Bad Q9 number")))</f>
         <v>0</v>
       </c>
       <c r="F4" s="5">
-        <f>MOD((HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]])) + ((HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) + IF(HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) &lt; HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]), 1440, 0) - (HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]))) / 2), 1440)</f>
+        <f>IF(OR(ISBLANK(data[[#This Row],[question_2]]), ISBLANK(data[[#This Row],[question_3]])), "", MOD((HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]])) + ((HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) + IF(HOUR(data[[#This Row],[question_3]])*60 + MINUTE(data[[#This Row],[question_3]]) &lt; HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]), 1440, 0) - (HOUR(data[[#This Row],[question_2]])*60 + MINUTE(data[[#This Row],[question_2]]))) / 2), 1440))</f>
         <v>900</v>
       </c>
       <c r="G4" s="5">
-        <f>MOD((HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]])) + ((HOUR(data[[#This Row],[question_6]])*60 + MINUTE(data[[#This Row],[question_6]]) + IF(HOUR(data[[#This Row],[question_6]])*60 + MINUTE(data[[#This Row],[question_6]]) &lt; HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]]), 1440, 0) - (HOUR(data[[#This Row],[question_5]])*60 + MINUTE(data[[#This Row],[question_5]]))) / 2), 1440)</f>
+        <f>IF(OR(ISBLANK(data[[#This Row],[question_5]]),ISBLANK(data[[#This Row],[question_6]])),"",MOD((HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]]))+((HOUR(data[[#This Row],[question_6]])*60+MINUTE(data[[#This Row],[question_6]])+IF(HOUR(data[[#This Row],[question_6]])*60+MINUTE(data[[#This Row],[question_6]])&lt;HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]]),1440,0)-(HOUR(data[[#This Row],[question_5]])*60+MINUTE(data[[#This Row],[question_5]])))/2),1440))</f>
         <v>480</v>
       </c>
       <c r="H4" s="5">
-        <f>IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=45, Table2[[#This Row],[weekday_mp]]&gt;=255), 0, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=60, Table2[[#This Row],[weekday_mp]]&gt;=240), 1, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=75, Table2[[#This Row],[weekday_mp]]&gt;=225), 2, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=90, Table2[[#This Row],[weekday_mp]]&gt;=210), 3, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=105, Table2[[#This Row],[weekday_mp]]&gt;=195), 4, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=120, Table2[[#This Row],[weekday_mp]]&gt;=180), 5, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=135, Table2[[#This Row],[weekday_mp]]&gt;=165), 6, 7)))))))</f>
+        <f>IF(ISBLANK(Table2[[#This Row],[weekday_mp]]), "", IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=45, Table2[[#This Row],[weekday_mp]]&gt;=255), 0, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=60, Table2[[#This Row],[weekday_mp]]&gt;=240), 1, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=75, Table2[[#This Row],[weekday_mp]]&gt;=225), 2, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=90, Table2[[#This Row],[weekday_mp]]&gt;=210), 3, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=105, Table2[[#This Row],[weekday_mp]]&gt;=195), 4, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=120, Table2[[#This Row],[weekday_mp]]&gt;=180), 5, IF(OR(Table2[[#This Row],[weekday_mp]]&lt;=135, Table2[[#This Row],[weekday_mp]]&gt;=165), 6, 7))))))))</f>
         <v>0</v>
       </c>
       <c r="I4" s="5" cm="1">
-        <f t="array" ref="I4">_xlfn.IFS(ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=90, 0, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=60, 1, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=30, 2, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&lt;30, 3)</f>
+        <f t="array" ref="I4">IF(OR(ISBLANK(Table2[[#This Row],[weekday_mp]]), ISBLANK(Table2[[#This Row],[weekend_mp]])), "", _xlfn.IFS(ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=90, 0, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=60, 1, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&gt;=30, 2, ABS(Table2[[#This Row],[weekday_mp]]-Table2[[#This Row],[weekend_mp]])&lt;30, 3))</f>
         <v>0</v>
       </c>
       <c r="J4" s="6" cm="1">
-        <f t="array" ref="J4">_xlfn.IFS(ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=120, 0, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=90, 1, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=60, 2, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=30, 3, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&lt;30, 4)</f>
+        <f t="array" ref="J4">IF(OR(ISBLANK(data[[#This Row],[question_4]]),ISBLANK(data[[#This Row],[question_7]])),"",_xlfn.IFS(ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=120, 0, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=90, 1, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=60, 2, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&gt;=30, 3, ABS(HOUR(data[[#This Row],[question_4]])*60+MINUTE(data[[#This Row],[question_4]])-HOUR(data[[#This Row],[question_7]])*60+MINUTE(data[[#This Row],[question_7]]))&lt;30, 4))</f>
         <v>0</v>
       </c>
       <c r="K4" s="3" cm="1">
-        <f t="array" ref="K4">_xlfn.IFS(data[[#This Row],[question_1]]=0, 0, data[[#This Row],[question_1]]=1, 10, data[[#This Row],[question_1]]=2, 5)</f>
+        <f t="array" ref="K4">IF(ISBLANK(data[[#This Row],[question_1]]), "", _xlfn.IFS(data[[#This Row],[question_1]]=0, 0, data[[#This Row],[question_1]]=1, 10, data[[#This Row],[question_1]]=2, 5))</f>
         <v>0</v>
       </c>
       <c r="L4" s="3">
-        <f>Table2[[#This Row],[q4_recoded]]+Table2[[#This Row],[q7_recoded]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[q4_recoded]], Table2[[#This Row],[q7_recoded]])=2, Table2[[#This Row],[q4_recoded]] + Table2[[#This Row],[q7_recoded]], "")</f>
         <v>0</v>
       </c>
       <c r="M4" s="3">
-        <f>Table2[[#This Row],[q8_recoded]]+Table2[[#This Row],[q9_recoded]]+Table2[[#This Row],[midpoint_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[q8_recoded]], Table2[[#This Row],[q9_recoded]], Table2[[#This Row],[midpoint_score]])=3, Table2[[#This Row],[q8_recoded]] + Table2[[#This Row],[q9_recoded]] + Table2[[#This Row],[midpoint_score]], "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="4">
-        <f>Table2[[#This Row],[social_jetlag_score]]+Table2[[#This Row],[sleep_duration_discrepancy_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[social_jetlag_score]], Table2[[#This Row],[sleep_duration_discrepancy_score]])=2, Table2[[#This Row],[social_jetlag_score]] + Table2[[#This Row],[sleep_duration_discrepancy_score]], "")</f>
         <v>0</v>
       </c>
       <c r="O4" s="3">
-        <f>(data[[#This Row],[question_10]])+(data[[#This Row],[question_14]])+(3-data[[#This Row],[question_15]])</f>
+        <f>IF(COUNTA(data[[#This Row],[question_10]], data[[#This Row],[question_14]], data[[#This Row],[question_15]])=3, (data[[#This Row],[question_10]]) + (data[[#This Row],[question_14]]) + (3-data[[#This Row],[question_15]]), "")</f>
         <v>0</v>
       </c>
       <c r="P4" s="3">
-        <f>(3-data[[#This Row],[question_11]])+(3-data[[#This Row],[question_12]])+(3-data[[#This Row],[question_13]])</f>
+        <f>IF(COUNTA(data[[#This Row],[question_11]], data[[#This Row],[question_12]], data[[#This Row],[question_13]])=3, (3-data[[#This Row],[question_11]]) + (3-data[[#This Row],[question_12]]) + (3-data[[#This Row],[question_13]]), "")</f>
         <v>0</v>
       </c>
       <c r="Q4" s="2">
-        <f>Table2[[#This Row],[problem_score]]+Table2[[#This Row],[duration_score]]+Table2[[#This Row],[timing_score]]+Table2[[#This Row],[regularity_score]]+Table2[[#This Row],[adequacy_score]]+Table2[[#This Row],[insomnia_score]]</f>
+        <f>IF(COUNTA(Table2[[#This Row],[problem_score]], Table2[[#This Row],[duration_score]], Table2[[#This Row],[timing_score]], Table2[[#This Row],[regularity_score]], Table2[[#This Row],[adequacy_score]], Table2[[#This Row],[insomnia_score]])=6, Table2[[#This Row],[problem_score]]+Table2[[#This Row],[duration_score]]+Table2[[#This Row],[timing_score]]+Table2[[#This Row],[regularity_score]]+Table2[[#This Row],[adequacy_score]]+Table2[[#This Row],[insomnia_score]], "")</f>
         <v>0</v>
       </c>
     </row>
@@ -1548,11 +1572,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>